<commit_message>
220413 COS Pro 1급 추가
</commit_message>
<xml_diff>
--- a/박진형 일정.xlsx
+++ b/박진형 일정.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dailyStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8C9632-4CB8-4C8D-A99B-0F114CE1D21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028A70A2-298B-424E-8C51-3563F3D3FE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6523" uniqueCount="3208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6549" uniqueCount="3216">
   <si>
     <t>6</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -14674,6 +14674,51 @@
   <si>
     <t>5시 E13 Future Lounge
 IAU 신규 전입자 간담회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>정봉현, 노숙진 생일
+고대치기공, 지산고 회비 입금
+7시반 신논현 류재열, 이승배</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>송포갈비 - 혜장국
+11시30분
+웨스턴 조선호텔 셔블 예약</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>저녁 6시 혜화 박용현, 윤석원
+도토리편백집-이마쇼쿠-
+리춘시장-노원 용현이형 집</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>신의주 순대국 - 메가커피</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>19시 마곡나루 icst 모임
+크라운호프
+20시반 에어부산 김포-&gt;김해</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>경주 교리김밥 - 페이지나인 -
+한화리조트 경주콘도
+예약번호 9295</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>보문호 산책 - 라한셀렉트 -
+경주 원조콩국 - 장전동 집 -
+영남식육식당</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>오스테리아밀즈 - 월정교 -
+한화리조트</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -23710,6 +23755,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="A21:A36"/>
+    <mergeCell ref="A58:A73"/>
+    <mergeCell ref="A107:A124"/>
+    <mergeCell ref="A91:A105"/>
+    <mergeCell ref="A75:A89"/>
     <mergeCell ref="C51:E51"/>
     <mergeCell ref="A38:A56"/>
     <mergeCell ref="A126:A141"/>
@@ -23717,12 +23768,6 @@
     <mergeCell ref="A196:A210"/>
     <mergeCell ref="A180:A194"/>
     <mergeCell ref="A143:A159"/>
-    <mergeCell ref="A2:A19"/>
-    <mergeCell ref="A21:A36"/>
-    <mergeCell ref="A58:A73"/>
-    <mergeCell ref="A107:A124"/>
-    <mergeCell ref="A91:A105"/>
-    <mergeCell ref="A75:A89"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27422,11 +27467,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A187:A204"/>
-    <mergeCell ref="A171:A185"/>
-    <mergeCell ref="A155:A169"/>
-    <mergeCell ref="A139:A153"/>
-    <mergeCell ref="A123:A137"/>
     <mergeCell ref="A104:A121"/>
     <mergeCell ref="A88:A102"/>
     <mergeCell ref="A2:A16"/>
@@ -27434,6 +27474,11 @@
     <mergeCell ref="A34:A51"/>
     <mergeCell ref="A53:A70"/>
     <mergeCell ref="A72:A86"/>
+    <mergeCell ref="A187:A204"/>
+    <mergeCell ref="A171:A185"/>
+    <mergeCell ref="A155:A169"/>
+    <mergeCell ref="A139:A153"/>
+    <mergeCell ref="A123:A137"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -39398,11 +39443,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A197:A211"/>
-    <mergeCell ref="A181:A195"/>
-    <mergeCell ref="A165:A179"/>
-    <mergeCell ref="A148:A163"/>
-    <mergeCell ref="A127:A146"/>
     <mergeCell ref="A110:A125"/>
     <mergeCell ref="A94:A108"/>
     <mergeCell ref="A2:A16"/>
@@ -39410,6 +39450,11 @@
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="A52:A68"/>
     <mergeCell ref="A70:A92"/>
+    <mergeCell ref="A197:A211"/>
+    <mergeCell ref="A181:A195"/>
+    <mergeCell ref="A165:A179"/>
+    <mergeCell ref="A148:A163"/>
+    <mergeCell ref="A127:A146"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43354,10 +43399,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527D31B6-BD14-4EA0-BC45-97C235EBCC6E}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5"/>
@@ -44257,7 +44302,7 @@
         <v>3204</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="12" customFormat="1" ht="50.1" customHeight="1">
+    <row r="49" spans="1:14" s="12" customFormat="1" ht="50.1" customHeight="1">
       <c r="A49" s="226"/>
       <c r="B49" s="198"/>
       <c r="C49" s="198"/>
@@ -44269,7 +44314,7 @@
         <v>3205</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="12" customFormat="1" ht="35.1" customHeight="1">
+    <row r="50" spans="1:14" s="12" customFormat="1" ht="35.1" customHeight="1">
       <c r="A50" s="226"/>
       <c r="B50" s="179" t="s">
         <v>21</v>
@@ -44289,7 +44334,7 @@
       <c r="G50" s="171"/>
       <c r="H50" s="171"/>
     </row>
-    <row r="51" spans="1:8" s="12" customFormat="1" ht="50.1" customHeight="1">
+    <row r="51" spans="1:14" s="12" customFormat="1" ht="50.1" customHeight="1">
       <c r="A51" s="226"/>
       <c r="B51" s="198" t="s">
         <v>3206</v>
@@ -44303,7 +44348,7 @@
       <c r="G51" s="198"/>
       <c r="H51" s="198"/>
     </row>
-    <row r="52" spans="1:8" s="12" customFormat="1" ht="49.9" customHeight="1">
+    <row r="52" spans="1:14" s="12" customFormat="1" ht="49.9" customHeight="1">
       <c r="A52" s="227"/>
       <c r="B52" s="198" t="s">
         <v>2912</v>
@@ -44314,6 +44359,129 @@
       <c r="F52" s="198"/>
       <c r="G52" s="198"/>
       <c r="H52" s="198"/>
+    </row>
+    <row r="53" spans="1:14" s="12" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A53" s="195" t="s">
+        <v>802</v>
+      </c>
+      <c r="B53" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="196" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="196" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="196" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="196" t="s">
+        <v>5</v>
+      </c>
+      <c r="G53" s="196" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="196" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" s="12" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A54" s="193"/>
+      <c r="B54" s="172"/>
+      <c r="C54" s="173"/>
+      <c r="D54" s="174"/>
+      <c r="E54" s="171"/>
+      <c r="F54" s="171"/>
+      <c r="G54" s="194" t="s">
+        <v>89</v>
+      </c>
+      <c r="H54" s="194" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" s="12" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A55" s="193"/>
+      <c r="B55" s="198"/>
+      <c r="C55" s="198"/>
+      <c r="D55" s="198"/>
+      <c r="E55" s="198"/>
+      <c r="F55" s="198"/>
+      <c r="G55" s="198" t="s">
+        <v>3208</v>
+      </c>
+      <c r="H55" s="198" t="s">
+        <v>3087</v>
+      </c>
+      <c r="N55" s="189"/>
+    </row>
+    <row r="56" spans="1:14" s="12" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A56" s="193"/>
+      <c r="B56" s="198"/>
+      <c r="C56" s="198"/>
+      <c r="D56" s="198"/>
+      <c r="E56" s="198"/>
+      <c r="F56" s="198"/>
+      <c r="G56" s="198" t="s">
+        <v>3209</v>
+      </c>
+      <c r="H56" s="198" t="s">
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" s="12" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A57" s="193"/>
+      <c r="B57" s="179" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="194" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" s="194" t="s">
+        <v>29</v>
+      </c>
+      <c r="E57" s="194" t="s">
+        <v>0</v>
+      </c>
+      <c r="F57" s="194" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57" s="194" t="s">
+        <v>30</v>
+      </c>
+      <c r="H57" s="194" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" s="12" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A58" s="193"/>
+      <c r="B58" s="198" t="s">
+        <v>3211</v>
+      </c>
+      <c r="C58" s="198"/>
+      <c r="D58" s="198"/>
+      <c r="E58" s="198"/>
+      <c r="F58" s="198" t="s">
+        <v>3212</v>
+      </c>
+      <c r="G58" s="198" t="s">
+        <v>3213</v>
+      </c>
+      <c r="H58" s="198" t="s">
+        <v>3214</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" s="12" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A59" s="193"/>
+      <c r="B59" s="198"/>
+      <c r="C59" s="198"/>
+      <c r="D59" s="198"/>
+      <c r="E59" s="198"/>
+      <c r="F59" s="198"/>
+      <c r="G59" s="198" t="s">
+        <v>3215</v>
+      </c>
+      <c r="H59" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>